<commit_message>
Manutenção nos campos do app.py
</commit_message>
<xml_diff>
--- a/projeto_expedicao/base_dados/155_010925.XLSX
+++ b/projeto_expedicao/base_dados/155_010925.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ambiente de Trabalho\Projetos\Projetos_Profissionais\Ativos\Projeto_BV_Pisos\Projeto_Inventário\projeto_expedicao\base_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{95BA7805-AD9E-4A74-850A-DE6E58D0A453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A578C60-5B2C-4763-9862-41E382860A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6151792F-F457-4F60-BF2F-9B8C8B8C3463}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6151792F-F457-4F60-BF2F-9B8C8B8C3463}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -1519,10 +1519,25 @@
   <dimension ref="A1:M204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M204"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>